<commit_message>
The rest of the changes (#3)
* Warrior tree changes

* Magic tree changes

* Defensive perk changes

* Toxin tree changes

* Assassin Perk Tree changes

* Elf changes

* MiscPerkChanges

* Change affixes and add new files

* Rework elderlicht braziers

* Medal updates

* More medal changes

* Fix some issues with xmls

* Attempt some fixes

* Add building definitions, clean up stuff that's not working

* Some weapon updates

* UpdateStuff

* Fix issue with script

* More_Changes

* Fix greataxe variants

* Fixes for enemies and usables

* Change stuff

* Final changes before the DLC
</commit_message>
<xml_diff>
--- a/scripts/WeaponData/tls_weapon_docs.xlsx
+++ b/scripts/WeaponData/tls_weapon_docs.xlsx
@@ -40,10 +40,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
-    <author>tc={d9a0c2b1-2ec7-497a-ba0d-d618b2a7a955}</author>
+    <author>tc={371ff404-2fb1-4aa2-aaf3-434418dc2a20}</author>
   </authors>
   <commentList>
-    <comment authorId="0" xr:uid="{d9a0c2b1-2ec7-497a-ba0d-d618b2a7a955}" ref="A18">
+    <comment authorId="0" xr:uid="{371ff404-2fb1-4aa2-aaf3-434418dc2a20}" ref="A18">
       <text>
         <t xml:space="preserve">[Threaded comment]
  Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -66,40 +66,13 @@
 <file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
-    <author>tc={4c2968f0-7e27-4c00-b81f-46f877ec43b2}</author>
-    <author>tc={a054324d-f8b5-4521-a1e6-3071cc4d1db5}</author>
-    <author>tc={bb41c8af-1522-4ab4-a4ed-f3cd1d163c13}</author>
-    <author>tc={f765dfdd-e6de-4ae9-9707-fb0efddc7749}</author>
+    <author>tc={26fa238d-bab2-4f32-b4fb-3e2d9285102e}</author>
+    <author>tc={85b6a0fa-5e46-4f28-993f-66c78b007f7d}</author>
+    <author>tc={c5ddd9ab-1abd-4520-ab63-4559a977c6cd}</author>
+    <author>tc={f4ff782d-cc13-4846-90f1-036446639059}</author>
   </authors>
   <commentList>
-    <comment authorId="0" xr:uid="{4c2968f0-7e27-4c00-b81f-46f877ec43b2}" ref="C16">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
- Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-	I think it could reduce armor or resistance as well as move instead of extra damage
-Reply:
-	This is only to compensate for the damage nerf really, I think the skill itself is fine. 10 targets is a lot.
-</t>
-      </text>
-    </comment>
-    <comment authorId="1" xr:uid="{a054324d-f8b5-4521-a1e6-3071cc4d1db5}" ref="B16">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
- Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-	I think the opportunism fits here
-Reply:
-	Maybe, but i put opportunism on assassinate instead. This is basically a strict buff, since 0.7 * 1.25 = 0.875
-Reply:
-	it can't have 2 sources of opportunitism like power staff?
-Reply:
-	Power staff has 1 opp skill, only skill 3
-It can have 2 anyway but I think it'll feel better with only 1.
-</t>
-      </text>
-    </comment>
-    <comment authorId="2" xr:uid="{bb41c8af-1522-4ab4-a4ed-f3cd1d163c13}" ref="D16">
+    <comment authorId="0" xr:uid="{26fa238d-bab2-4f32-b4fb-3e2d9285102e}" ref="D16">
       <text>
         <t xml:space="preserve">[Threaded comment]
  Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -117,7 +90,34 @@
 </t>
       </text>
     </comment>
-    <comment authorId="3" xr:uid="{f765dfdd-e6de-4ae9-9707-fb0efddc7749}" ref="A16">
+    <comment authorId="1" xr:uid="{85b6a0fa-5e46-4f28-993f-66c78b007f7d}" ref="C16">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+ Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+	I think it could reduce armor or resistance as well as move instead of extra damage
+Reply:
+	This is only to compensate for the damage nerf really, I think the skill itself is fine. 10 targets is a lot.
+</t>
+      </text>
+    </comment>
+    <comment authorId="2" xr:uid="{c5ddd9ab-1abd-4520-ab63-4559a977c6cd}" ref="B16">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+ Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+	I think the opportunism fits here
+Reply:
+	Maybe, but i put opportunism on assassinate instead. This is basically a strict buff, since 0.7 * 1.25 = 0.875
+Reply:
+	it can't have 2 sources of opportunitism like power staff?
+Reply:
+	Power staff has 1 opp skill, only skill 3
+It can have 2 anyway but I think it'll feel better with only 1.
+</t>
+      </text>
+    </comment>
+    <comment authorId="3" xr:uid="{f4ff782d-cc13-4846-90f1-036446639059}" ref="A16">
       <text>
         <t xml:space="preserve">[Threaded comment]
  Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -138,10 +138,10 @@
 <file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
-    <author>tc={e3c72fb1-beb0-42f2-aabc-19fa50078fc0}</author>
+    <author>tc={5ff03feb-1ab4-466a-8075-9e901beb6cec}</author>
   </authors>
   <commentList>
-    <comment authorId="0" xr:uid="{e3c72fb1-beb0-42f2-aabc-19fa50078fc0}" ref="D17">
+    <comment authorId="0" xr:uid="{5ff03feb-1ab4-466a-8075-9e901beb6cec}" ref="D17">
       <text>
         <t xml:space="preserve">[Threaded comment]
  Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -167,10 +167,10 @@
 <file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
-    <author>tc={46df504f-ed7a-4c47-8ed3-6b7cfb702c41}</author>
+    <author>tc={7ccf6dc5-7bdf-44dc-80d4-5d2c8e115a19}</author>
   </authors>
   <commentList>
-    <comment authorId="0" xr:uid="{46df504f-ed7a-4c47-8ed3-6b7cfb702c41}" ref="B18">
+    <comment authorId="0" xr:uid="{7ccf6dc5-7bdf-44dc-80d4-5d2c8e115a19}" ref="B18">
       <text>
         <t xml:space="preserve">[Threaded comment]
  Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -189,10 +189,10 @@
 <file path=xl/comments13.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
-    <author>tc={e00ed579-bc11-427a-8a9b-2f2ee78f5373}</author>
+    <author>tc={bf025aea-7664-4f5c-bb22-e7b51fe9542d}</author>
   </authors>
   <commentList>
-    <comment authorId="0" xr:uid="{e00ed579-bc11-427a-8a9b-2f2ee78f5373}" ref="D16">
+    <comment authorId="0" xr:uid="{bf025aea-7664-4f5c-bb22-e7b51fe9542d}" ref="D16">
       <text>
         <t xml:space="preserve">[Threaded comment]
  Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -218,10 +218,10 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
-    <author>tc={0fb32eca-7a23-413c-a91c-ca48b26f8570}</author>
+    <author>tc={88520c76-5f3c-4c61-9141-f8d3f33405b7}</author>
   </authors>
   <commentList>
-    <comment authorId="0" xr:uid="{0fb32eca-7a23-413c-a91c-ca48b26f8570}" ref="D18">
+    <comment authorId="0" xr:uid="{88520c76-5f3c-4c61-9141-f8d3f33405b7}" ref="D18">
       <text>
         <t xml:space="preserve">[Threaded comment]
  Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -252,10 +252,10 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
-    <author>tc={0684cfee-faee-4ffd-bdf1-725be1a35a8c}</author>
+    <author>tc={d99ae072-43cc-4b5b-8072-d772c53cf673}</author>
   </authors>
   <commentList>
-    <comment authorId="0" xr:uid="{0684cfee-faee-4ffd-bdf1-725be1a35a8c}" ref="B15">
+    <comment authorId="0" xr:uid="{d99ae072-43cc-4b5b-8072-d772c53cf673}" ref="B15">
       <text>
         <t xml:space="preserve">[Threaded comment]
  Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -273,10 +273,10 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
-    <author>tc={170d76aa-3afd-4879-a8d0-2866af125d98}</author>
+    <author>tc={392286e5-b497-46ab-b1e3-68fca29816e2}</author>
   </authors>
   <commentList>
-    <comment authorId="0" xr:uid="{170d76aa-3afd-4879-a8d0-2866af125d98}" ref="A18">
+    <comment authorId="0" xr:uid="{392286e5-b497-46ab-b1e3-68fca29816e2}" ref="A18">
       <text>
         <t xml:space="preserve">[Threaded comment]
  Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -302,11 +302,23 @@
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
-    <author>tc={1033cc30-37a8-4f25-a43d-bfc96893ee5f}</author>
-    <author>tc={9d660cc8-a511-45cd-981f-f454f69252f4}</author>
+    <author>tc={79521f8f-d8ac-4e66-bb26-c0781b010b1d}</author>
+    <author>tc={9f02fb39-bd03-4bf6-b3cc-d8ce91f714f2}</author>
   </authors>
   <commentList>
-    <comment authorId="0" xr:uid="{1033cc30-37a8-4f25-a43d-bfc96893ee5f}" ref="C22">
+    <comment authorId="0" xr:uid="{79521f8f-d8ac-4e66-bb26-c0781b010b1d}" ref="B18">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+ Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+	I'm not sure about the -dodge if it's really necessary.
+would be possible to increase the skills damage by block amount?
+Reply:
+	I think it's worthwhile if we're removing base stat penalties from weapons, but tbh yes, it's not needed and we can just keep the -flat dodge. I don't think it's possible to increase the skills damage by the block amount, the perk already kind of does something like that anyway.
+</t>
+      </text>
+    </comment>
+    <comment authorId="1" xr:uid="{9f02fb39-bd03-4bf6-b3cc-d8ce91f714f2}" ref="C22">
       <text>
         <t xml:space="preserve">[Threaded comment]
  Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -322,18 +334,6 @@
 </t>
       </text>
     </comment>
-    <comment authorId="1" xr:uid="{9d660cc8-a511-45cd-981f-f454f69252f4}" ref="B18">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
- Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-	I'm not sure about the -dodge if it's really necessary.
-would be possible to increase the skills damage by block amount?
-Reply:
-	I think it's worthwhile if we're removing base stat penalties from weapons, but tbh yes, it's not needed and we can just keep the -flat dodge. I don't think it's possible to increase the skills damage by the block amount, the perk already kind of does something like that anyway.
-</t>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -341,11 +341,11 @@
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
-    <author>tc={2ba21228-6298-4981-bb94-faef1d843e51}</author>
-    <author>tc={a5d624f7-0af1-477c-a87e-e94265ff5d8d}</author>
+    <author>tc={5efeeaea-176c-4160-b85d-5239256bb7bd}</author>
+    <author>tc={6d733127-4a2e-4534-ad7b-0f260bb1a39f}</author>
   </authors>
   <commentList>
-    <comment authorId="0" xr:uid="{2ba21228-6298-4981-bb94-faef1d843e51}" ref="B17">
+    <comment authorId="0" xr:uid="{5efeeaea-176c-4160-b85d-5239256bb7bd}" ref="B17">
       <text>
         <t xml:space="preserve">[Threaded comment]
  Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -368,7 +368,7 @@
 </t>
       </text>
     </comment>
-    <comment authorId="1" xr:uid="{a5d624f7-0af1-477c-a87e-e94265ff5d8d}" ref="A17">
+    <comment authorId="1" xr:uid="{6d733127-4a2e-4534-ad7b-0f260bb1a39f}" ref="A17">
       <text>
         <t xml:space="preserve">[Threaded comment]
  Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -393,10 +393,10 @@
 <file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
-    <author>tc={0aa10fe6-9711-422a-ae6c-1e6fb1c8dda6}</author>
+    <author>tc={48cd5993-c932-48dc-95d3-6fa64ed4f8ed}</author>
   </authors>
   <commentList>
-    <comment authorId="0" xr:uid="{0aa10fe6-9711-422a-ae6c-1e6fb1c8dda6}" ref="A18">
+    <comment authorId="0" xr:uid="{48cd5993-c932-48dc-95d3-6fa64ed4f8ed}" ref="A18">
       <text>
         <t xml:space="preserve">[Threaded comment]
  Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -424,10 +424,10 @@
 <file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
-    <author>tc={8aa7e893-116a-4eb9-9d18-1c2bc4970dbf}</author>
+    <author>tc={23e26434-87c4-4283-b33e-edaeeeb8c05a}</author>
   </authors>
   <commentList>
-    <comment authorId="0" xr:uid="{8aa7e893-116a-4eb9-9d18-1c2bc4970dbf}" ref="C16">
+    <comment authorId="0" xr:uid="{23e26434-87c4-4283-b33e-edaeeeb8c05a}" ref="C16">
       <text>
         <t xml:space="preserve">[Threaded comment]
  Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -453,10 +453,10 @@
 <file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
-    <author>tc={4a61c193-336a-4e67-aca1-f2099a06d4d2}</author>
+    <author>tc={d6cffc4c-72e9-462b-8eb6-43ea04b520ff}</author>
   </authors>
   <commentList>
-    <comment authorId="0" xr:uid="{4a61c193-336a-4e67-aca1-f2099a06d4d2}" ref="A16">
+    <comment authorId="0" xr:uid="{d6cffc4c-72e9-462b-8eb6-43ea04b520ff}" ref="A16">
       <text>
         <t xml:space="preserve">[Threaded comment]
  Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -477,7 +477,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="193">
   <si>
     <t>These are the weapon variant values for Tier 1 weapon variants, so Steel, Silver, Journeyman's and Adepts</t>
   </si>
@@ -743,7 +743,7 @@
     <t>Now has a 3x3 aoe, centered around the bottom-center tile</t>
   </si>
   <si>
-    <t>dmg mod to 1.45x from 1.4x</t>
+    <t>dmg mod to 1.6x from 1.4x</t>
   </si>
   <si>
     <t>New skill 2 aoe</t>
@@ -797,9 +797,6 @@
     <t>accuracy</t>
   </si>
   <si>
-    <t>daily hp regen</t>
-  </si>
-  <si>
     <t>reliability</t>
   </si>
   <si>
@@ -815,6 +812,12 @@
     <t>dmg mod to 1.15x</t>
   </si>
   <si>
+    <t>dmg mod decreased to 1.05x from 1.1x</t>
+  </si>
+  <si>
+    <t>dmg mod decreased to 1.1x from 1.2x</t>
+  </si>
+  <si>
     <t>physical damage</t>
   </si>
   <si>
@@ -863,14 +866,11 @@
     <t>isolation</t>
   </si>
   <si>
-    <t>Reworked to: a skill: Slow death, 1ap, deals base damage and inflicts 60 additional poison for 3 turns. 4 uses per turn</t>
-  </si>
-  <si>
-    <t>Reworked to: Quickshot: 1 ap, 3 multihits
-2 uses, inaccurate 2x</t>
-  </si>
-  <si>
-    <t>Added a 1.25x opportunist multiplier</t>
+    <t>Reworked to: a skill: Slow death, 1ap, deals base damage and inflicts 45 additional poison for 2 turns. 4 uses per turn</t>
+  </si>
+  <si>
+    <t>Reworked to: Quickshot: 2 ap, 3 multihits
+2 uses, inaccurate 2x, 1.25x damage modifier</t>
   </si>
   <si>
     <t>poison damage</t>
@@ -933,7 +933,7 @@
     <t>switches places with skill 1, Dmg mod to 1.0x, no longer has opportunism multiplier</t>
   </si>
   <si>
-    <t>Reworked to: 2 uses, 1 ap 2 mana, 2 move points, damage mod: 1.25x, 1.5x isolation multiplier, 1.5x opportunism multiplier, undodgeable.</t>
+    <t>Reworked to: 2 uses, 1 ap 2 mana, 2 move points, damage mod: 1.0x, 1.5x isolation multiplier, 1.5x opportunism multiplier, undodgeable.</t>
   </si>
   <si>
     <t>Remove the -1 move speed</t>
@@ -981,7 +981,7 @@
     <t>No longer grants a damage buff, purges all debuffs from target</t>
   </si>
   <si>
-    <t>dmg mod 0.75x, 5 base multihits</t>
+    <t>dmg mod to 0.8x from 0.85x, 5 base multihits</t>
   </si>
   <si>
     <t>Journeyman</t>
@@ -1014,7 +1014,7 @@
     <t>DMG mod to 1.35x</t>
   </si>
   <si>
-    <t>DMG mod to 1.6x</t>
+    <t>DMG mod to 1.6x, base propagation bounces to 9</t>
   </si>
   <si>
     <t>magic damage</t>
@@ -1805,9 +1805,9 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <x18tc:personList xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments">
-  <x18tc:person displayName="Grobo bobo" id="{78ec551f-0095-45a7-93a1-2d270a4fc022}" providerId="google-sheets"/>
-  <x18tc:person displayName="Abigail" id="{87f3b5a7-bddc-49a0-8964-c62ea7f071e4}" providerId="google-sheets"/>
-  <x18tc:person displayName="ellaris clavis" id="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" providerId="google-sheets"/>
+  <x18tc:person displayName="Grobo bobo" id="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" providerId="google-sheets"/>
+  <x18tc:person displayName="Abigail" id="{bd03cfe2-7f11-4fc0-96f7-fa6c96340b6b}" providerId="google-sheets"/>
+  <x18tc:person displayName="ellaris clavis" id="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" providerId="google-sheets"/>
 </x18tc:personList>
 </file>
 
@@ -2480,16 +2480,16 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <x18tc:ThreadedComments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <x18tc:threadedComment ref="A18" dT="2026-01-18T15:45:42.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{d9a0c2b1-2ec7-497a-ba0d-d618b2a7a955}" done="1">
+  <x18tc:threadedComment ref="A18" dT="2026-01-18T15:45:42.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{371ff404-2fb1-4aa2-aaf3-434418dc2a20}" done="1">
     <x18tc:text xml:space="preserve">This feels like it makes the hammer a ranged weapon</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="A18" dT="2026-01-18T16:37:24.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{5139ff14-aaf4-498a-95d8-1daa4188608b}" parentId="{d9a0c2b1-2ec7-497a-ba0d-d618b2a7a955}">
+  <x18tc:threadedComment ref="A18" dT="2026-01-18T16:37:24.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{276fbb85-e2cb-45ed-bdf1-5d780744bb84}" parentId="{371ff404-2fb1-4aa2-aaf3-434418dc2a20}">
     <x18tc:text xml:space="preserve">Why? do you mean the +1 use on the skill 2?</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="A18" dT="2026-01-18T17:38:03.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{d6f2aeb5-a1f2-4e40-8cf8-73479e12bded}" parentId="{d9a0c2b1-2ec7-497a-ba0d-d618b2a7a955}">
+  <x18tc:threadedComment ref="A18" dT="2026-01-18T17:38:03.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{1ffe42b3-64f6-491f-878a-f01b9b89ea05}" parentId="{371ff404-2fb1-4aa2-aaf3-434418dc2a20}">
     <x18tc:text xml:space="preserve">yes, moving from skill 1 into 2, also skill 2 is already quite strong, I think maybe skill 3 could have something to help with killing those enemies, like  2 turn armor or resistance debuff alongside the stun</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="A18" dT="2026-01-18T19:16:53.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{dce78284-3443-47ff-b040-039c72dd69e5}" parentId="{d9a0c2b1-2ec7-497a-ba0d-d618b2a7a955}">
+  <x18tc:threadedComment ref="A18" dT="2026-01-18T19:16:53.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{e3369b81-31dd-4ada-b156-31cde91d73f8}" parentId="{371ff404-2fb1-4aa2-aaf3-434418dc2a20}">
     <x18tc:text xml:space="preserve">Okay, that's fair, I'm reverting the skill use changes. 
 Skill 3 is mostly about stun, so it doesn't need help killing the side tiles though.</x18tc:text>
   </x18tc:threadedComment>
@@ -2498,46 +2498,46 @@
 
 <file path=xl/threadedComments/threadedComment10.xml><?xml version="1.0" encoding="utf-8"?>
 <x18tc:ThreadedComments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <x18tc:threadedComment ref="C16" dT="2026-01-18T15:55:31.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{4c2968f0-7e27-4c00-b81f-46f877ec43b2}" done="1">
+  <x18tc:threadedComment ref="C16" dT="2026-01-18T15:55:31.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{85b6a0fa-5e46-4f28-993f-66c78b007f7d}" done="1">
     <x18tc:text xml:space="preserve">I think it could reduce armor or resistance as well as move instead of extra damage</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="C16" dT="2026-01-18T16:46:04.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{a084d99b-63aa-435c-ab57-c1acc099c6c8}" parentId="{4c2968f0-7e27-4c00-b81f-46f877ec43b2}">
+  <x18tc:threadedComment ref="C16" dT="2026-01-18T16:46:04.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{9a3f54ab-2d1e-4383-8411-d9e669eaaa0a}" parentId="{85b6a0fa-5e46-4f28-993f-66c78b007f7d}">
     <x18tc:text xml:space="preserve">This is only to compensate for the damage nerf really, I think the skill itself is fine. 10 targets is a lot.</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="D16" dT="2026-01-18T16:00:36.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{bb41c8af-1522-4ab4-a4ed-f3cd1d163c13}" done="0">
+  <x18tc:threadedComment ref="D16" dT="2026-01-18T16:00:36.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{26fa238d-bab2-4f32-b4fb-3e2d9285102e}" done="0">
     <x18tc:text xml:space="preserve">I would keep it at 1 use and high cost, just make sure it kills whatever it targets, with high damage, I would even say it should have high damage multiplayer and like 80-90% isolation + opportunitism effectiveness</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="D16" dT="2026-01-18T16:48:57.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{f5216a81-83fb-459a-a58c-2f379ee93a2f}" parentId="{bb41c8af-1522-4ab4-a4ed-f3cd1d163c13}">
+  <x18tc:threadedComment ref="D16" dT="2026-01-18T16:48:57.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{bb0f0e9d-b233-4294-85cc-7859c66c0fca}" parentId="{26fa238d-bab2-4f32-b4fb-3e2d9285102e}">
     <x18tc:text xml:space="preserve">Keeping it 2 ap and 1 use Makes it far, far worse than the scroll variant. I intend to rework it into a high-effort, more costly but also a lot more damaging snipe shot, and making it 2 ap would just make it worse than snipe shot.</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="D16" dT="2026-01-18T17:29:52.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{0969f002-4444-4d79-afb1-016a9ad990ba}" parentId="{bb41c8af-1522-4ab4-a4ed-f3cd1d163c13}">
+  <x18tc:threadedComment ref="D16" dT="2026-01-18T17:29:52.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{a107b2f3-d69d-456c-8d3e-f0006df3bc7c}" parentId="{26fa238d-bab2-4f32-b4fb-3e2d9285102e}">
     <x18tc:text xml:space="preserve">yeah, asssasinate just sounds quite heavy and so does rifle, it just feels like it's beccomming more of a prickle shot.
 It sounds like it should be good against hight hp enemies like elites, which you might not meet 2 off.
 but I think assassinate sounds better if you don't have to put that much work into it?</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="D16" dT="2026-01-18T19:15:23.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{236931d9-e999-4eb9-bb98-9d3cf4e268ae}" parentId="{bb41c8af-1522-4ab4-a4ed-f3cd1d163c13}">
+  <x18tc:threadedComment ref="D16" dT="2026-01-18T19:15:23.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{ec3f6889-dbf7-408e-a1b4-7bf32f1e52c8}" parentId="{26fa238d-bab2-4f32-b4fb-3e2d9285102e}">
     <x18tc:text xml:space="preserve">What do you mean prickle shot? It's a pretty major damage buff compared to what we had previously.
 I think setting up assassination is pretty thematic personally, and that's where the heaviness can come from.</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="A16" dT="2026-01-18T15:57:43.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{f765dfdd-e6de-4ae9-9707-fb0efddc7749}" done="1">
+  <x18tc:threadedComment ref="A16" dT="2026-01-18T15:57:43.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{f4ff782d-cc13-4846-90f1-036446639059}" done="1">
     <x18tc:text xml:space="preserve">is this also instead of the new propagation?
 I think undogeable makes sense since it's a high cost skill, maybe secondary targets for damage or debuff (armor/dodge/resistance)?</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="A16" dT="2026-01-18T16:44:29.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{05f9b455-5db3-4e16-8d9f-0d9617d6849f}" parentId="{f765dfdd-e6de-4ae9-9707-fb0efddc7749}">
+  <x18tc:threadedComment ref="A16" dT="2026-01-18T16:44:29.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{ac7d6e07-7340-4474-ac81-ab0e86956bb2}" parentId="{f4ff782d-cc13-4846-90f1-036446639059}">
     <x18tc:text xml:space="preserve">No, it's with the new propagation, and the assumption that it loses the -prop damage debuff
 I removed undodgeable to put it on assassinate, as it really needs it
 I think armor piercing is a stronger modifier than undodgeable, especially for this skill</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="B16" dT="2026-01-18T15:57:59.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{a054324d-f8b5-4521-a1e6-3071cc4d1db5}" done="0">
+  <x18tc:threadedComment ref="B16" dT="2026-01-18T15:57:59.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{c5ddd9ab-1abd-4520-ab63-4559a977c6cd}" done="0">
     <x18tc:text xml:space="preserve">I think the opportunism fits here</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="B16" dT="2026-01-18T16:45:26.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{30b69ecd-ed27-4b91-a0ad-cc028ce4d2db}" parentId="{a054324d-f8b5-4521-a1e6-3071cc4d1db5}">
+  <x18tc:threadedComment ref="B16" dT="2026-01-18T16:45:26.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{0a4f5285-6d49-410d-8e1b-1324f1322c62}" parentId="{c5ddd9ab-1abd-4520-ab63-4559a977c6cd}">
     <x18tc:text xml:space="preserve">Maybe, but i put opportunism on assassinate instead. This is basically a strict buff, since 0.7 * 1.25 = 0.875</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="B16" dT="2026-01-18T18:40:17.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{a36d3eca-a1ff-43a6-a90e-30cad0601fcc}" parentId="{a054324d-f8b5-4521-a1e6-3071cc4d1db5}">
+  <x18tc:threadedComment ref="B16" dT="2026-01-18T18:40:17.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{50a824fe-cd50-4595-a49d-e1f2e65239e1}" parentId="{c5ddd9ab-1abd-4520-ab63-4559a977c6cd}">
     <x18tc:text xml:space="preserve">it can't have 2 sources of opportunitism like power staff?</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="B16" dT="2026-01-18T19:25:30.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{287dbd25-8b6e-49fd-a224-0f1a4f9b132a}" parentId="{a054324d-f8b5-4521-a1e6-3071cc4d1db5}">
+  <x18tc:threadedComment ref="B16" dT="2026-01-18T19:25:30.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{24f2a26b-d39a-4285-9487-e0a5d7377315}" parentId="{c5ddd9ab-1abd-4520-ab63-4559a977c6cd}">
     <x18tc:text xml:space="preserve">Power staff has 1 opp skill, only skill 3
 It can have 2 anyway but I think it'll feel better with only 1.</x18tc:text>
   </x18tc:threadedComment>
@@ -2546,20 +2546,20 @@
 
 <file path=xl/threadedComments/threadedComment11.xml><?xml version="1.0" encoding="utf-8"?>
 <x18tc:ThreadedComments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <x18tc:threadedComment ref="D17" dT="2026-01-18T16:09:42.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{e3c72fb1-beb0-42f2-aabc-19fa50078fc0}" done="1">
+  <x18tc:threadedComment ref="D17" dT="2026-01-18T16:09:42.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{5ff03feb-1ab4-466a-8075-9e901beb6cec}" done="1">
     <x18tc:text xml:space="preserve">don't understand/unfinished
 what if you removed damage from all skills, and have the perk deal damage to all stunned targets within range at the end of turn (when the boomerang  comes back)?</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="D17" dT="2026-01-18T16:52:32.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{32e3373e-9f02-4cfc-ac00-77edce2cf39d}" parentId="{e3c72fb1-beb0-42f2-aabc-19fa50078fc0}">
+  <x18tc:threadedComment ref="D17" dT="2026-01-18T16:52:32.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{a8847601-2508-4daa-a9ee-ba22987b0a8c}" parentId="{5ff03feb-1ab4-466a-8075-9e901beb6cec}">
     <x18tc:text xml:space="preserve">My bad, was meant to be "After the hero stuns 3 enemies, boomerang's side tiles become main tiles"
 I want to get rid of the ricochet entirely because it makes it feel like it plays the game for you. Removing damage from all skills would double down on that feeling.</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="D17" dT="2026-01-18T18:36:18.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{33b5e7c0-edc7-49e6-83e1-3c527a3d3c8e}" parentId="{e3c72fb1-beb0-42f2-aabc-19fa50078fc0}">
+  <x18tc:threadedComment ref="D17" dT="2026-01-18T18:36:18.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{2fcb029e-0706-41e4-9a13-193d4eda4f11}" parentId="{5ff03feb-1ab4-466a-8075-9e901beb6cec}">
     <x18tc:text xml:space="preserve">so you would have to use skill 1 before using skills 2 and 3 (if it's only 1 use that would be horrible?)
 I don't know, doesn't sound exciting.
 Also you remove multihit and propagation and not add anything, sounds weak.</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="D17" dT="2026-01-18T19:34:58.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{f693c290-59b2-46d1-bbde-d2418458d61a}" parentId="{e3c72fb1-beb0-42f2-aabc-19fa50078fc0}">
+  <x18tc:threadedComment ref="D17" dT="2026-01-18T19:34:58.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{4245a45d-4c33-4d79-ae25-232040613b22}" parentId="{5ff03feb-1ab4-466a-8075-9e901beb6cec}">
     <x18tc:text xml:space="preserve">no, you can still stun with skills 2 and 3, or other sources. And while i did remove prop, i added damage, quite a lot of it in fact. I don't think skill 3 with 1.75x damage mod and like 20 targets is weak. or 1 ap 1 mana 7 targets 1.6 damage mod. The most similar weapon to it would probably be gauntlet i think.</x18tc:text>
   </x18tc:threadedComment>
 </x18tc:ThreadedComments>
@@ -2567,10 +2567,10 @@
 
 <file path=xl/threadedComments/threadedComment12.xml><?xml version="1.0" encoding="utf-8"?>
 <x18tc:ThreadedComments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <x18tc:threadedComment ref="B18" dT="2026-01-18T16:12:45.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{46df504f-ed7a-4c47-8ed3-6b7cfb702c41}" done="0">
+  <x18tc:threadedComment ref="B18" dT="2026-01-18T16:12:45.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{7ccf6dc5-7bdf-44dc-80d4-5d2c8e115a19}" done="0">
     <x18tc:text xml:space="preserve">I would just make the buff skill have higher range, increase momentum and scale movement 2/3/4/5</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="B18" dT="2026-01-18T16:56:30.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{667fa561-b6ff-44a8-9edd-299bbf5d1779}" parentId="{46df504f-ed7a-4c47-8ed3-6b7cfb702c41}">
+  <x18tc:threadedComment ref="B18" dT="2026-01-18T16:56:30.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{cd3ab098-2082-4c31-a710-c43fc37f4bcf}" parentId="{7ccf6dc5-7bdf-44dc-80d4-5d2c8e115a19}">
     <x18tc:text xml:space="preserve">So you want to nerf it early? It already grants 3 movement at tier 0. 
 The big problem with wind walk is that its boring, already covered by a trinket skill, and basically worse than transfer as a support skill. Shocking touch is a scepter's old skill that's already in the game files, and I think it'll be a better fit for the weapon. But if it turns out to be bad, why not, we'll bring back wind walk.</x18tc:text>
   </x18tc:threadedComment>
@@ -2579,20 +2579,20 @@
 
 <file path=xl/threadedComments/threadedComment13.xml><?xml version="1.0" encoding="utf-8"?>
 <x18tc:ThreadedComments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <x18tc:threadedComment ref="D16" dT="2026-01-18T16:16:57.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{e00ed579-bc11-427a-8a9b-2f2ee78f5373}" done="0">
+  <x18tc:threadedComment ref="D16" dT="2026-01-18T16:16:57.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{bf025aea-7664-4f5c-bb22-e7b51fe9542d}" done="0">
     <x18tc:text xml:space="preserve">not sure the change to skill 3 is enough maybe it should deal damage to the center tile,
 still feels like skill 4 is too strong, and anti synergistic by dealing damage and applying poison</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="D16" dT="2026-01-18T16:58:44.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{bb2517a7-ebc9-460d-b1fb-629061bb9d28}" parentId="{e00ed579-bc11-427a-8a9b-2f2ee78f5373}">
+  <x18tc:threadedComment ref="D16" dT="2026-01-18T16:58:44.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{d19fd80f-bbcb-4b3a-a32b-7f662c9f40f2}" parentId="{bf025aea-7664-4f5c-bb22-e7b51fe9542d}">
     <x18tc:text xml:space="preserve">The skill 3 debuff is underrated, as demonstrated already by longbow's skill 2, it was just too expensive
 I think bee sting is fine, Why do you think applying damage and poison is anti-synergistic? it's perfectly fine.</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="D16" dT="2026-01-18T17:20:15.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{cefd6f9d-3ac2-48ae-bf7b-ad32a733555a}" parentId="{e00ed579-bc11-427a-8a9b-2f2ee78f5373}">
+  <x18tc:threadedComment ref="D16" dT="2026-01-18T17:20:15.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{da6b6a7d-0912-4329-a87b-a9fb6118d1ba}" parentId="{bf025aea-7664-4f5c-bb22-e7b51fe9542d}">
     <x18tc:text xml:space="preserve">if you get +poison or just +damage you buff only half of the skill, similar with other stats/perks that affects damage or poison/debuffs.
 you want to apply poison to go through the enemies armor, but you deal enough damage to break that armor or the resistant guy just dies and doesn't get the poison.
 It's kind of if a skill did some ranged damage and then it also did some physical damage, the benefit of doing physical damage (armor breaking) would go to waste</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="D16" dT="2026-01-18T17:29:49.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{b6cbf157-fd26-41ee-8a78-14c72ce155fa}" parentId="{e00ed579-bc11-427a-8a9b-2f2ee78f5373}">
+  <x18tc:threadedComment ref="D16" dT="2026-01-18T17:29:49.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{0aaf234c-8bb3-4d83-bc47-c4e1ee7940f1}" parentId="{bf025aea-7664-4f5c-bb22-e7b51fe9542d}">
     <x18tc:text xml:space="preserve">That's less anti-synergy and more just normal lack of synergy. Some damage can get wasted but it's not harmful. Not every enemy has armor. It's also just common enough to not be a big deal.</x18tc:text>
   </x18tc:threadedComment>
 </x18tc:ThreadedComments>
@@ -2600,28 +2600,28 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <x18tc:ThreadedComments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <x18tc:threadedComment ref="D18" dT="2026-01-18T15:48:47.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{0fb32eca-7a23-413c-a91c-ca48b26f8570}" done="1">
+  <x18tc:threadedComment ref="D18" dT="2026-01-18T15:48:47.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{88520c76-5f3c-4c61-9141-f8d3f33405b7}" done="1">
     <x18tc:text xml:space="preserve">not sure if this is enough to make it feel good?
 at least make skill 1 able to target ground</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="D18" dT="2026-01-18T16:39:59.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{df816f03-1f58-4411-ac4a-f4d6f84caf66}" parentId="{0fb32eca-7a23-413c-a91c-ca48b26f8570}">
+  <x18tc:threadedComment ref="D18" dT="2026-01-18T16:39:59.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{9d6cdafc-db4b-4976-951b-1ebf90d111f6}" parentId="{88520c76-5f3c-4c61-9141-f8d3f33405b7}">
     <x18tc:text xml:space="preserve">I think it should be enough
 Maybe skill 2 should also get more base momentum, but 2h sword is already pretty close to being good.
 I'm not sure if it's possible to make 2h sword ground targetable but it's worth looking into</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="D18" dT="2026-01-18T17:06:03.00" personId="{87f3b5a7-bddc-49a0-8964-c62ea7f071e4}" id="{85507cc7-17b9-4bff-ab50-4dd5576a408d}" parentId="{0fb32eca-7a23-413c-a91c-ca48b26f8570}">
+  <x18tc:threadedComment ref="D18" dT="2026-01-18T17:06:03.00" personId="{bd03cfe2-7f11-4fc0-96f7-fa6c96340b6b}" id="{81ce1d0d-aab9-4a6b-8705-632d3d53f463}" parentId="{88520c76-5f3c-4c61-9141-f8d3f33405b7}">
     <x18tc:text xml:space="preserve">the movement cost on skill 4 is my biggest criticism of 2h sword, so this is a change I agree with</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="D18" dT="2026-01-18T17:36:04.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{d8ca5428-0c08-45e0-83b1-0bdf1ff573ae}" parentId="{0fb32eca-7a23-413c-a91c-ca48b26f8570}">
+  <x18tc:threadedComment ref="D18" dT="2026-01-18T17:36:04.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{d8804813-7137-489d-8c2e-5d5e7b575521}" parentId="{88520c76-5f3c-4c61-9141-f8d3f33405b7}">
     <x18tc:text xml:space="preserve">it does feel bad, since it's hard to position, adn you already pay for momentum with movement, and if you're short you have to use skill 1 which makes skill 4 do less damage (if you kill)</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="D18" dT="2026-01-18T18:07:44.00" personId="{87f3b5a7-bddc-49a0-8964-c62ea7f071e4}" id="{3ec354c3-0a70-45dc-bd50-57fbd5ab8d65}" parentId="{0fb32eca-7a23-413c-a91c-ca48b26f8570}">
+  <x18tc:threadedComment ref="D18" dT="2026-01-18T18:07:44.00" personId="{bd03cfe2-7f11-4fc0-96f7-fa6c96340b6b}" id="{8da74f22-3a0c-4ea0-b706-2c43a737de4a}" parentId="{88520c76-5f3c-4c61-9141-f8d3f33405b7}">
     <x18tc:text xml:space="preserve">Skill 1 doesn't change the damage of skill 4? And why would killing with it matter?</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="D18" dT="2026-01-18T18:41:53.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{8e77b80a-df57-442b-b487-18cc0efb81b2}" parentId="{0fb32eca-7a23-413c-a91c-ca48b26f8570}">
+  <x18tc:threadedComment ref="D18" dT="2026-01-18T18:41:53.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{0b57f7fc-66e0-4d62-9aad-54f6b2dd0bdd}" parentId="{88520c76-5f3c-4c61-9141-f8d3f33405b7}">
     <x18tc:text xml:space="preserve">what I meant is if you end up in a place where you don't have enough movement for skill 4, and need to use skill 1 to get the movement, and kill enemies you wanted to target with skill 4, it feels bad</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="D18" dT="2026-01-18T18:47:50.00" personId="{87f3b5a7-bddc-49a0-8964-c62ea7f071e4}" id="{9071e7de-b7fe-49a5-92fa-09d7e1c240de}" parentId="{0fb32eca-7a23-413c-a91c-ca48b26f8570}">
+  <x18tc:threadedComment ref="D18" dT="2026-01-18T18:47:50.00" personId="{bd03cfe2-7f11-4fc0-96f7-fa6c96340b6b}" id="{615ea674-0bd9-4215-8258-e02a329dea8f}" parentId="{88520c76-5f3c-4c61-9141-f8d3f33405b7}">
     <x18tc:text xml:space="preserve">And that will happen less if skill 4 doesn't cost movement?</x18tc:text>
   </x18tc:threadedComment>
 </x18tc:ThreadedComments>
@@ -2629,10 +2629,10 @@
 
 <file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
 <x18tc:ThreadedComments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <x18tc:threadedComment ref="B15" dT="2026-01-18T17:17:55.00" personId="{87f3b5a7-bddc-49a0-8964-c62ea7f071e4}" id="{0684cfee-faee-4ffd-bdf1-725be1a35a8c}" done="1">
+  <x18tc:threadedComment ref="B15" dT="2026-01-18T17:17:55.00" personId="{bd03cfe2-7f11-4fc0-96f7-fa6c96340b6b}" id="{d99ae072-43cc-4b5b-8072-d772c53cf673}" done="1">
     <x18tc:text xml:space="preserve">I'd also make it apply the debuff to the main target tile</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="B15" dT="2026-01-18T17:30:14.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{57c6cbc8-f01a-4622-ac42-88827dc81b89}" parentId="{0684cfee-faee-4ffd-bdf1-725be1a35a8c}">
+  <x18tc:threadedComment ref="B15" dT="2026-01-18T17:30:14.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{5db39c4f-6a3a-497b-a103-8d62d8720834}" parentId="{d99ae072-43cc-4b5b-8072-d772c53cf673}">
     <x18tc:text xml:space="preserve">Sure</x18tc:text>
   </x18tc:threadedComment>
 </x18tc:ThreadedComments>
@@ -2640,20 +2640,20 @@
 
 <file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
 <x18tc:ThreadedComments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <x18tc:threadedComment ref="A18" dT="2026-01-18T15:53:30.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{170d76aa-3afd-4879-a8d0-2866af125d98}" done="1">
+  <x18tc:threadedComment ref="A18" dT="2026-01-18T15:53:30.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{392286e5-b497-46ab-b1e3-68fca29816e2}" done="1">
     <x18tc:text xml:space="preserve">I don't think this would be very helpful.
 Maybe a x3 multihit (and slightly lower damage) with range 1-2 non-modifiable?
 probably would need to change skill 3 away from multihit tho, like a cardinal spear throw with higher range, and maybe secondary damage on the sides (or debuff)</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="A18" dT="2026-01-18T16:42:08.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{8270ecc5-a38b-43b2-a353-eb4325147103}" parentId="{170d76aa-3afd-4879-a8d0-2866af125d98}">
+  <x18tc:threadedComment ref="A18" dT="2026-01-18T16:42:08.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{984fd661-11c7-48e5-9af8-26551b338506}" parentId="{392286e5-b497-46ab-b1e3-68fca29816e2}">
     <x18tc:text xml:space="preserve">Why would this not be helpful? the issue of this skill is that 3 targets is too little for the damage it deals, adding a 4th would change a lot. If it's too weak, it can be a full tile instead of a side tile, but i think that could be too strong considering how good the spear already is
 I'm definitely not adding any MH to a skill 1 :P</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="A18" dT="2026-01-18T17:34:42.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{cd3069a9-7383-471b-bc8d-81308a941236}" parentId="{170d76aa-3afd-4879-a8d0-2866af125d98}">
+  <x18tc:threadedComment ref="A18" dT="2026-01-18T17:34:42.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{7f055ab6-fa56-4cf7-9d5a-25626f089346}" parentId="{392286e5-b497-46ab-b1e3-68fca29816e2}">
     <x18tc:text xml:space="preserve">that is fine, but it could be more balanced on a melee weapon.
 The idea is that it is starting to look like great axe with different shape, and I think great age works better since you can stay in the middle of the wave, where as with the spear it could be better from the side?</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="A18" dT="2026-01-18T19:20:21.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{23d3c102-3d58-42b4-a51b-d1525d26f610}" parentId="{170d76aa-3afd-4879-a8d0-2866af125d98}">
+  <x18tc:threadedComment ref="A18" dT="2026-01-18T19:20:21.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{a4397647-a63d-4adb-85b6-c5fa88255ede}" parentId="{392286e5-b497-46ab-b1e3-68fca29816e2}">
     <x18tc:text xml:space="preserve">Yeah, the damage, positioning, amount of tiles, and accuracy is still different so i think it's different enough.</x18tc:text>
   </x18tc:threadedComment>
 </x18tc:ThreadedComments>
@@ -2661,24 +2661,24 @@
 
 <file path=xl/threadedComments/threadedComment5.xml><?xml version="1.0" encoding="utf-8"?>
 <x18tc:ThreadedComments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <x18tc:threadedComment ref="B18" dT="2026-01-18T15:00:09.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{9d660cc8-a511-45cd-981f-f454f69252f4}" done="1">
+  <x18tc:threadedComment ref="B18" dT="2026-01-18T15:00:09.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{79521f8f-d8ac-4e66-bb26-c0781b010b1d}" done="1">
     <x18tc:text xml:space="preserve">I'm not sure about the -dodge if it's really necessary.
 would be possible to increase the skills damage by block amount?</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="B18" dT="2026-01-18T15:32:34.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{53e41025-7626-42e5-87b2-f1f2a7d081db}" parentId="{9d660cc8-a511-45cd-981f-f454f69252f4}">
+  <x18tc:threadedComment ref="B18" dT="2026-01-18T15:32:34.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{62d77798-cd3d-45d4-8bd2-ee53ee1ff169}" parentId="{79521f8f-d8ac-4e66-bb26-c0781b010b1d}">
     <x18tc:text xml:space="preserve">I think it's worthwhile if we're removing base stat penalties from weapons, but tbh yes, it's not needed and we can just keep the -flat dodge. I don't think it's possible to increase the skills damage by the block amount, the perk already kind of does something like that anyway.</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="C22" dT="2026-01-18T15:02:54.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{1033cc30-37a8-4f25-a43d-bfc96893ee5f}" done="1">
+  <x18tc:threadedComment ref="C22" dT="2026-01-18T15:02:54.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{9f02fb39-bd03-4bf6-b3cc-d8ce91f714f2}" done="1">
     <x18tc:text xml:space="preserve">could make the steel grant block and this one give movement, since it's light and you like to position yourself with it</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="C22" dT="2026-01-18T15:33:33.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{7c41c260-e46f-4738-b5c4-b9734d425896}" parentId="{1033cc30-37a8-4f25-a43d-bfc96893ee5f}">
+  <x18tc:threadedComment ref="C22" dT="2026-01-18T15:33:33.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{75c21ccc-7a55-4b96-84ea-ed1877766d15}" parentId="{9f02fb39-bd03-4bf6-b3cc-d8ce91f714f2}">
     <x18tc:text xml:space="preserve">That's an option, although few weapons make sense with +armor, so i wanted war shield to have it.</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="C22" dT="2026-01-18T17:47:05.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{bdabcd8b-d3f3-4d3a-8f59-fdfeec98ff06}" parentId="{1033cc30-37a8-4f25-a43d-bfc96893ee5f}">
+  <x18tc:threadedComment ref="C22" dT="2026-01-18T17:47:05.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{60b5e73d-76b9-48b0-8ee6-79ab766b09f6}" parentId="{9f02fb39-bd03-4bf6-b3cc-d8ce91f714f2}">
     <x18tc:text xml:space="preserve">It would make most sense to be on shield, but I would still prefer to keep armor on my armor.
 also is the amount at tier 5? because it might not be that great, is tier 5 supposed to block an attack or half from a regular clawer?</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="C22" dT="2026-01-18T19:19:02.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{0a92a9bc-4856-44f7-acd9-8e6200504904}" parentId="{1033cc30-37a8-4f25-a43d-bfc96893ee5f}">
+  <x18tc:threadedComment ref="C22" dT="2026-01-18T19:19:02.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{7e778cc2-658d-4221-a748-165e4697e6c4}" parentId="{9f02fb39-bd03-4bf6-b3cc-d8ce91f714f2}">
     <x18tc:text xml:space="preserve">No, we start calculating from tier 0</x18tc:text>
   </x18tc:threadedComment>
 </x18tc:ThreadedComments>
@@ -2686,40 +2686,40 @@
 
 <file path=xl/threadedComments/threadedComment6.xml><?xml version="1.0" encoding="utf-8"?>
 <x18tc:ThreadedComments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <x18tc:threadedComment ref="A17" dT="2026-01-18T16:17:52.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{a5d624f7-0af1-477c-a87e-e94265ff5d8d}" done="1">
+  <x18tc:threadedComment ref="A17" dT="2026-01-18T16:17:52.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{6d733127-4a2e-4534-ad7b-0f260bb1a39f}" done="1">
     <x18tc:text xml:space="preserve">I don't think dealing damage and applying poison at the same time makes too much sense</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="A17" dT="2026-01-18T16:50:22.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{670b5dbf-e537-4e9b-8e65-3713d91c9006}" parentId="{a5d624f7-0af1-477c-a87e-e94265ff5d8d}">
+  <x18tc:threadedComment ref="A17" dT="2026-01-18T16:50:22.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{32487dbb-23f1-4772-a401-3cc0d69e62f3}" parentId="{6d733127-4a2e-4534-ad7b-0f260bb1a39f}">
     <x18tc:text xml:space="preserve">Why not? Orb does it, Sacred flower does it, bee sting does it.</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="A17" dT="2026-01-18T17:08:00.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{20bcc6af-51a2-49d4-a1f6-9c09370d6002}" parentId="{a5d624f7-0af1-477c-a87e-e94265ff5d8d}">
+  <x18tc:threadedComment ref="A17" dT="2026-01-18T17:08:00.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{57da634b-85a9-4743-b2c3-c6298aadc95d}" parentId="{6d733127-4a2e-4534-ad7b-0f260bb1a39f}">
     <x18tc:text xml:space="preserve">Also dagger skill 3 does it</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="A17" dT="2026-01-18T17:10:54.00" personId="{87f3b5a7-bddc-49a0-8964-c62ea7f071e4}" id="{8b818c23-aaee-46a9-ae03-782b2ea1d41b}" parentId="{a5d624f7-0af1-477c-a87e-e94265ff5d8d}">
+  <x18tc:threadedComment ref="A17" dT="2026-01-18T17:10:54.00" personId="{bd03cfe2-7f11-4fc0-96f7-fa6c96340b6b}" id="{c7648cf6-702d-4d2c-9451-91214b11e92f}" parentId="{6d733127-4a2e-4534-ad7b-0f260bb1a39f}">
     <x18tc:text xml:space="preserve">yeah, it makes the skills a little worse than if they just do poison, because the poison doesn't get applied if the enemy dies or dodges, but that's just a balancing factor
 And Hand crossbow doesn't need skills that ignore even more defensive stats</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="A17" dT="2026-01-18T19:28:34.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{ea3477f5-6135-45fe-bdcd-772fcbf903cf}" parentId="{a5d624f7-0af1-477c-a87e-e94265ff5d8d}">
+  <x18tc:threadedComment ref="A17" dT="2026-01-18T19:28:34.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{33f0623c-4435-4447-80e0-9984bc291497}" parentId="{6d733127-4a2e-4534-ad7b-0f260bb1a39f}">
     <x18tc:text xml:space="preserve">I think the skill will remain fine, keeping it unchanged for now.</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="B17" dT="2026-01-18T16:06:10.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{2ba21228-6298-4981-bb94-faef1d843e51}" done="0">
+  <x18tc:threadedComment ref="B17" dT="2026-01-18T16:06:10.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{5efeeaea-176c-4160-b85d-5239256bb7bd}" done="1">
     <x18tc:text xml:space="preserve">how about -1 movement instead of mana for 2 multihits and 3 uses?
 or start the ability with 2 multihit and higher multiplayer on lowe item tier and 3 multihit with lower multiplayer on higher tier?
 I don't think there is a very clean way for 1 ap multihit</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="B17" dT="2026-01-18T16:34:13.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{75fff16c-646d-480e-a1e2-3111b5dd2f50}" parentId="{2ba21228-6298-4981-bb94-faef1d843e51}">
+  <x18tc:threadedComment ref="B17" dT="2026-01-18T16:34:13.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{0ad15b68-f77a-426e-a099-e9d6002e6c74}" parentId="{5efeeaea-176c-4160-b85d-5239256bb7bd}">
     <x18tc:text xml:space="preserve">No, Making it 3 MH base but 2 uses is very, very important, it's what's gonna balance it without making it terrible early. MH was busted with xbow due to each MH being +50% damage, and it having a lot of uses. Higher base MH and lower uses is the point.
 I disagree on it being unclean, I think it's pretty clean, the inaccurate and opp multiplier effects are optional and mostly for flavor, can remove them if you don't like them. It costing mana is also optional tbh
 I could make it manaless but lose the +opp modifier.</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="B17" dT="2026-01-18T17:12:01.00" personId="{87f3b5a7-bddc-49a0-8964-c62ea7f071e4}" id="{72a23701-87a4-4980-9434-cc9b7cf1b4fd}" parentId="{2ba21228-6298-4981-bb94-faef1d843e51}">
+  <x18tc:threadedComment ref="B17" dT="2026-01-18T17:12:01.00" personId="{bd03cfe2-7f11-4fc0-96f7-fa6c96340b6b}" id="{a539b648-05b3-4784-887c-fe5aa13bfb17}" parentId="{5efeeaea-176c-4160-b85d-5239256bb7bd}">
     <x18tc:text xml:space="preserve">I think manaless but no opp would be better, it feels weird for a non magic weapon to use mana on skill 2
 but yeah, 2 uses is the important balancing aspect</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="B17" dT="2026-01-18T17:24:17.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{f07f3f16-d997-474d-9ec9-9a22a0ae4643}" parentId="{2ba21228-6298-4981-bb94-faef1d843e51}">
+  <x18tc:threadedComment ref="B17" dT="2026-01-18T17:24:17.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{41d016b5-0d9c-43e5-a43f-7289528e6906}" parentId="{5efeeaea-176c-4160-b85d-5239256bb7bd}">
     <x18tc:text xml:space="preserve">yeah, I can see that, it might also be that it looks like it doesn't know what to do since it can use any stat, maybe it should just focus on doing 1 thing instead of being able to do everything?</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="B17" dT="2026-01-18T19:27:21.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{f67ca292-c65f-4761-a565-ac6226c90e17}" parentId="{2ba21228-6298-4981-bb94-faef1d843e51}">
+  <x18tc:threadedComment ref="B17" dT="2026-01-18T19:27:21.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{ac4e898a-32a9-46fe-a05f-c31954a7a6af}" parentId="{5efeeaea-176c-4160-b85d-5239256bb7bd}">
     <x18tc:text xml:space="preserve">That's why i tried to give it opp, to focus more on the debuff/poison
 But I've removed opp and mana cost, and gave opp to blaze instead.</x18tc:text>
   </x18tc:threadedComment>
@@ -2728,24 +2728,24 @@
 
 <file path=xl/threadedComments/threadedComment7.xml><?xml version="1.0" encoding="utf-8"?>
 <x18tc:ThreadedComments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <x18tc:threadedComment ref="A18" dT="2026-01-18T15:09:00.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{0aa10fe6-9711-422a-ae6c-1e6fb1c8dda6}" done="0">
+  <x18tc:threadedComment ref="A18" dT="2026-01-18T15:09:00.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{48cd5993-c932-48dc-95d3-6fa64ed4f8ed}" done="0">
     <x18tc:text xml:space="preserve">I kinda liked the old one, not a fan of these changes</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="A18" dT="2026-01-18T15:30:26.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{55209434-1c2b-4d7d-a5e4-06604d899cff}" parentId="{0aa10fe6-9711-422a-ae6c-1e6fb1c8dda6}">
+  <x18tc:threadedComment ref="A18" dT="2026-01-18T15:30:26.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{693fe7da-d190-4be7-8bca-52db578b59ce}" parentId="{48cd5993-c932-48dc-95d3-6fa64ed4f8ed}">
     <x18tc:text xml:space="preserve">I can revert the skill 2 and 4 changes but I do think the -res debuff should go to the hammer, not crossbow</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="A18" dT="2026-01-18T17:07:25.00" personId="{87f3b5a7-bddc-49a0-8964-c62ea7f071e4}" id="{6ab97670-d03c-419c-b289-f1b16c1cffdf}" parentId="{0aa10fe6-9711-422a-ae6c-1e6fb1c8dda6}">
+  <x18tc:threadedComment ref="A18" dT="2026-01-18T17:07:25.00" personId="{bd03cfe2-7f11-4fc0-96f7-fa6c96340b6b}" id="{18194931-1b52-4c67-8595-4f17bde721bd}" parentId="{48cd5993-c932-48dc-95d3-6fa64ed4f8ed}">
     <x18tc:text xml:space="preserve">I almost think that crossbow just doesn't need any debuffs. Debuffs and using opportunism doesn't need to be something that every single weapon can do?</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="A18" dT="2026-01-18T17:27:25.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{62d6c93f-bfa8-42f9-9bec-c0c347d78d23}" parentId="{0aa10fe6-9711-422a-ae6c-1e6fb1c8dda6}">
+  <x18tc:threadedComment ref="A18" dT="2026-01-18T17:27:25.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{ce11bde3-7b7a-4235-8289-89a7fdd1556e}" parentId="{48cd5993-c932-48dc-95d3-6fa64ed4f8ed}">
     <x18tc:text xml:space="preserve">It does not need it, but since i want to put the -res on hammer i do think it could use something
 It's generally fun if skills 1 and 2 have some spice.  I can always just increase the base damage of it further instead.</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="A18" dT="2026-01-18T17:44:12.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{72b09bab-9937-4909-9bbb-468586b0812f}" parentId="{0aa10fe6-9711-422a-ae6c-1e6fb1c8dda6}">
+  <x18tc:threadedComment ref="A18" dT="2026-01-18T17:44:12.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{0faab1ef-dccc-4be9-a2bf-e03eef0e11f0}" parentId="{48cd5993-c932-48dc-95d3-6fa64ed4f8ed}">
     <x18tc:text xml:space="preserve">yeah, I thnk skill 2 shouldn't have isolation, it's the skill you use to make targets isolated since it has high damage, and it needs positioning, so it's harder to target isolated stragglers.
 I'm not much of a fan of skill 4 in general, could it be like a side by side triple skill 3 for double the cost? or maker it look like an arrow head, reverse of pistol skill</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="A18" dT="2026-01-18T19:23:51.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{e58d4aa8-21bd-4782-8a14-870b3823a6b4}" parentId="{0aa10fe6-9711-422a-ae6c-1e6fb1c8dda6}">
+  <x18tc:threadedComment ref="A18" dT="2026-01-18T19:23:51.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{db281b1d-79f5-4a77-91e3-2cda55b21e7f}" parentId="{48cd5993-c932-48dc-95d3-6fa64ed4f8ed}">
     <x18tc:text xml:space="preserve">Reverted the Skill 2 changes. As for skill 4, you have edit rights, so draw the aoe you're talking about. Though I'm not a fan of yet another grapeshot blast shape, we already have 3 of these</x18tc:text>
   </x18tc:threadedComment>
 </x18tc:ThreadedComments>
@@ -2753,22 +2753,22 @@
 
 <file path=xl/threadedComments/threadedComment8.xml><?xml version="1.0" encoding="utf-8"?>
 <x18tc:ThreadedComments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <x18tc:threadedComment ref="C16" dT="2026-01-18T16:01:26.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{8aa7e893-116a-4eb9-9d18-1c2bc4970dbf}" done="1">
+  <x18tc:threadedComment ref="C16" dT="2026-01-18T16:01:26.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{23e26434-87c4-4283-b33e-edaeeeb8c05a}" done="1">
     <x18tc:text xml:space="preserve">I feel like it might need more damage, unless base damage already covers that, but pistol always felt weak for me</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="C16" dT="2026-01-18T16:49:52.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{03e2ec71-c7f0-41c7-9366-81d3203ec1a0}" parentId="{8aa7e893-116a-4eb9-9d18-1c2bc4970dbf}">
+  <x18tc:threadedComment ref="C16" dT="2026-01-18T16:49:52.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{f7e6afc2-f8c2-497b-9464-ca7d0d539df1}" parentId="{23e26434-87c4-4283-b33e-edaeeeb8c05a}">
     <x18tc:text xml:space="preserve">I think the base damage covers that well enough. It's one of the better skill 3s anyway.</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="C16" dT="2026-01-18T17:09:06.00" personId="{87f3b5a7-bddc-49a0-8964-c62ea7f071e4}" id="{ac80fc57-6ee8-44f6-9b19-3890187029ae}" parentId="{8aa7e893-116a-4eb9-9d18-1c2bc4970dbf}">
+  <x18tc:threadedComment ref="C16" dT="2026-01-18T17:09:06.00" personId="{bd03cfe2-7f11-4fc0-96f7-fa6c96340b6b}" id="{6ca91ee5-c7ea-4779-aeb7-2654718cdb20}" parentId="{23e26434-87c4-4283-b33e-edaeeeb8c05a}">
     <x18tc:text xml:space="preserve">grape shot is a very good skill, a base damage increase would improve it early and then late game it becomes great with proximity shot</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="C16" dT="2026-01-18T17:26:05.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{40a3fa9e-689f-48e2-aee3-5c3ad20c81bd}" parentId="{8aa7e893-116a-4eb9-9d18-1c2bc4970dbf}">
+  <x18tc:threadedComment ref="C16" dT="2026-01-18T17:26:05.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{a9a6d36b-5161-47e2-ba71-2e7205cf0eea}" parentId="{23e26434-87c4-4283-b33e-edaeeeb8c05a}">
     <x18tc:text xml:space="preserve">yeah, I don't play with many "ranged" perks, since they tend to be ranged damage specific and kinda weird overall, the other perks are definitely more universal</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="C16" dT="2026-01-18T18:06:28.00" personId="{87f3b5a7-bddc-49a0-8964-c62ea7f071e4}" id="{d797013b-3447-4399-9914-484a097ccea4}" parentId="{8aa7e893-116a-4eb9-9d18-1c2bc4970dbf}">
+  <x18tc:threadedComment ref="C16" dT="2026-01-18T18:06:28.00" personId="{bd03cfe2-7f11-4fc0-96f7-fa6c96340b6b}" id="{32469f06-f2a6-4de6-a442-f741fc238260}" parentId="{23e26434-87c4-4283-b33e-edaeeeb8c05a}">
     <x18tc:text xml:space="preserve">Proximity shot is the only one that's ranged damage specific, and it's a very very good perk</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="C16" dT="2026-01-18T18:37:49.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{9e28503d-4633-4a3f-87a6-fae2fd7a8a18}" parentId="{8aa7e893-116a-4eb9-9d18-1c2bc4970dbf}">
+  <x18tc:threadedComment ref="C16" dT="2026-01-18T18:37:49.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{84a1e061-b6d3-4631-a8f2-eac1e0d7ce79}" parentId="{23e26434-87c4-4283-b33e-edaeeeb8c05a}">
     <x18tc:text xml:space="preserve">maybe it's just me who likes to kill enemies at range with ranged damage instead of in melee :p</x18tc:text>
   </x18tc:threadedComment>
 </x18tc:ThreadedComments>
@@ -2776,17 +2776,17 @@
 
 <file path=xl/threadedComments/threadedComment9.xml><?xml version="1.0" encoding="utf-8"?>
 <x18tc:ThreadedComments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <x18tc:threadedComment ref="A16" dT="2026-01-18T15:44:17.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{4a61c193-336a-4e67-aca1-f2099a06d4d2}" done="0">
+  <x18tc:threadedComment ref="A16" dT="2026-01-18T15:44:17.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{d6cffc4c-72e9-462b-8eb6-43ea04b520ff}" done="0">
     <x18tc:text xml:space="preserve">I don't like this change, I think it makes more sense to exchange the scattershot to longbow (since it's "inaccurate" at long range) and bring the arctic stun to shortbow and have skill 1 to be opportunistic.
 Have shortbow be a good horde killer and longbow be good at picking enemies off</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="A16" dT="2026-01-18T16:38:06.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{984c1960-5e3b-487e-b996-bf4d4363eab6}" parentId="{4a61c193-336a-4e67-aca1-f2099a06d4d2}">
+  <x18tc:threadedComment ref="A16" dT="2026-01-18T16:38:06.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{d51aafa1-eb8e-44aa-b239-1410f4bd2d6f}" parentId="{d6cffc4c-72e9-462b-8eb6-43ea04b520ff}">
     <x18tc:text xml:space="preserve">Long bow already has snipe shot for picking enemies off, and shortbow's skill 4 is literally about creating isolated targets. Giving shortbow arctic blast would also mean it has skill 3 and 4 that basically do the same thing, which is lame.</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="A16" dT="2026-01-18T17:39:51.00" personId="{1ecb0197-ddcf-4fcd-9a5d-7d54f877cfae}" id="{bc3ce2e5-c445-490e-b96d-3c96e7cf01ed}" parentId="{4a61c193-336a-4e67-aca1-f2099a06d4d2}">
+  <x18tc:threadedComment ref="A16" dT="2026-01-18T17:39:51.00" personId="{c1a868ca-8e0e-488c-9718-8347b8d8735b}" id="{47b2d83b-0c78-4bf7-b637-8862e2c414d6}" parentId="{d6cffc4c-72e9-462b-8eb6-43ea04b520ff}">
     <x18tc:text xml:space="preserve">but short bow can't pick enemies off since it has short range, that is why longbow is good at picking off stragglers, also you want to debuff a group of enemies to stop the from advancing so it would make sense to have shortbow have opportunism to finish those enemies off</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="A16" dT="2026-01-18T19:21:36.00" personId="{78ec551f-0095-45a7-93a1-2d270a4fc022}" id="{1a4fa5eb-efbc-466c-9c1f-bd83bef7f372}" parentId="{4a61c193-336a-4e67-aca1-f2099a06d4d2}">
+  <x18tc:threadedComment ref="A16" dT="2026-01-18T19:21:36.00" personId="{790c6c93-dac0-4b48-86e9-fe6213d8c276}" id="{9ae4c660-ed1c-4bcc-8b1f-93465240c738}" parentId="{d6cffc4c-72e9-462b-8eb6-43ea04b520ff}">
     <x18tc:text xml:space="preserve">Shortbow has 8 base range, that is not low. It also has only 1 use of a debuff skill compared to longbow's 4.</x18tc:text>
   </x18tc:threadedComment>
 </x18tc:ThreadedComments>
@@ -3310,7 +3310,7 @@
         <v>69</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" ht="16.5" customHeight="1">
@@ -3329,15 +3329,15 @@
       </c>
       <c r="E6" s="10">
         <f t="shared" ref="E6:E12" si="2">ROUND(F6*H6,0)</f>
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="F6" s="10">
         <f>ROUND(F7 * 0.9,0)</f>
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="G6" s="10">
         <f t="shared" ref="G6:G12" si="3">AVERAGE(E6:F6)</f>
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="H6" s="10">
         <v>0.8</v>
@@ -3359,14 +3359,14 @@
       </c>
       <c r="E7" s="10">
         <f t="shared" si="2"/>
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="F7" s="10">
-        <v>122.0</v>
+        <v>134.0</v>
       </c>
       <c r="G7" s="10">
         <f t="shared" si="3"/>
-        <v>110</v>
+        <v>120.5</v>
       </c>
       <c r="H7" s="10">
         <v>0.8</v>
@@ -3389,15 +3389,15 @@
       </c>
       <c r="E8" s="10">
         <f t="shared" si="2"/>
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="F8" s="10">
         <f t="shared" ref="F8:F12" si="4">ROUND(F7*1.1,0)</f>
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="G8" s="10">
         <f t="shared" si="3"/>
-        <v>120.5</v>
+        <v>132.5</v>
       </c>
       <c r="H8" s="10">
         <v>0.8</v>
@@ -3420,15 +3420,15 @@
       </c>
       <c r="E9" s="10">
         <f t="shared" si="2"/>
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="F9" s="10">
         <f t="shared" si="4"/>
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="G9" s="10">
         <f t="shared" si="3"/>
-        <v>132.5</v>
+        <v>146</v>
       </c>
       <c r="H9" s="10">
         <v>0.8</v>
@@ -3451,15 +3451,15 @@
       </c>
       <c r="E10" s="10">
         <f t="shared" si="2"/>
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="F10" s="10">
         <f t="shared" si="4"/>
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="G10" s="10">
         <f t="shared" si="3"/>
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="H10" s="10">
         <v>0.8</v>
@@ -3482,15 +3482,15 @@
       </c>
       <c r="E11" s="10">
         <f t="shared" si="2"/>
-        <v>142</v>
+        <v>157</v>
       </c>
       <c r="F11" s="10">
         <f t="shared" si="4"/>
-        <v>178</v>
+        <v>196</v>
       </c>
       <c r="G11" s="10">
         <f t="shared" si="3"/>
-        <v>160</v>
+        <v>176.5</v>
       </c>
       <c r="H11" s="10">
         <v>0.8</v>
@@ -3512,15 +3512,15 @@
       </c>
       <c r="E12" s="10">
         <f t="shared" si="2"/>
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="F12" s="10">
         <f t="shared" si="4"/>
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="G12" s="10">
         <f t="shared" si="3"/>
-        <v>176.5</v>
+        <v>194.5</v>
       </c>
       <c r="H12" s="10">
         <v>0.8</v>
@@ -3555,13 +3555,17 @@
     </row>
     <row r="18">
       <c r="A18" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="C18" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="29"/>
+      <c r="D18" s="29" t="s">
+        <v>112</v>
+      </c>
       <c r="K18" s="28"/>
       <c r="L18" s="28"/>
       <c r="P18" s="28"/>
@@ -3606,7 +3610,7 @@
     </row>
     <row r="22">
       <c r="A22" s="30" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B22" s="27" t="s">
         <v>7</v>
@@ -3615,7 +3619,7 @@
         <v>34</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H22" s="13"/>
     </row>
@@ -3928,7 +3932,7 @@
     </row>
     <row r="13">
       <c r="I13" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="L13" s="31"/>
       <c r="M13" s="31"/>
@@ -3964,7 +3968,7 @@
         <v>95</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>90</v>
@@ -3975,19 +3979,19 @@
         <v>84</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H18" s="33"/>
     </row>
@@ -4012,7 +4016,7 @@
     </row>
     <row r="22" ht="36.0" customHeight="1">
       <c r="A22" s="34" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B22" s="34" t="s">
         <v>8</v>
@@ -4021,7 +4025,7 @@
         <v>36</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -4345,7 +4349,7 @@
         <v>95</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16">
@@ -4353,7 +4357,7 @@
         <v>84</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>84</v>
@@ -4362,7 +4366,7 @@
         <v>84</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20">
@@ -4386,13 +4390,13 @@
     </row>
     <row r="22">
       <c r="A22" s="34" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B22" s="34" t="s">
         <v>15</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>35</v>
@@ -4512,15 +4516,15 @@
       </c>
       <c r="E6" s="10">
         <f t="shared" ref="E6:E12" si="2">ROUND(F6*H6,0)</f>
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="F6" s="10">
         <f>ROUND(F7 * 0.9,0)</f>
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="G6" s="10">
         <f t="shared" ref="G6:G12" si="3">AVERAGE(E6:F6)</f>
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="H6" s="10">
         <v>0.8</v>
@@ -4542,14 +4546,14 @@
       </c>
       <c r="E7" s="10">
         <f t="shared" si="2"/>
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="F7" s="10">
-        <v>65.0</v>
+        <v>76.0</v>
       </c>
       <c r="G7" s="10">
         <f t="shared" si="3"/>
-        <v>58.5</v>
+        <v>68.5</v>
       </c>
       <c r="H7" s="10">
         <v>0.8</v>
@@ -4571,15 +4575,15 @@
       </c>
       <c r="E8" s="10">
         <f t="shared" si="2"/>
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="F8" s="10">
         <f t="shared" ref="F8:F12" si="4">ROUND(F7*1.1,0)</f>
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="G8" s="10">
         <f t="shared" si="3"/>
-        <v>65</v>
+        <v>75.5</v>
       </c>
       <c r="H8" s="10">
         <v>0.8</v>
@@ -4601,15 +4605,15 @@
       </c>
       <c r="E9" s="10">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F9" s="10">
         <f t="shared" si="4"/>
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="G9" s="10">
         <f t="shared" si="3"/>
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="H9" s="10">
         <v>0.8</v>
@@ -4631,15 +4635,15 @@
       </c>
       <c r="E10" s="10">
         <f t="shared" si="2"/>
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="F10" s="10">
         <f t="shared" si="4"/>
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="G10" s="10">
         <f t="shared" si="3"/>
-        <v>78.5</v>
+        <v>91</v>
       </c>
       <c r="H10" s="10">
         <v>0.8</v>
@@ -4661,15 +4665,15 @@
       </c>
       <c r="E11" s="10">
         <f t="shared" si="2"/>
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="F11" s="10">
         <f t="shared" si="4"/>
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="G11" s="10">
         <f t="shared" si="3"/>
-        <v>86.5</v>
+        <v>100</v>
       </c>
       <c r="H11" s="10">
         <v>0.8</v>
@@ -4691,15 +4695,15 @@
       </c>
       <c r="E12" s="10">
         <f t="shared" si="2"/>
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="F12" s="10">
         <f t="shared" si="4"/>
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="G12" s="10">
         <f t="shared" si="3"/>
-        <v>95.5</v>
+        <v>110</v>
       </c>
       <c r="H12" s="10">
         <v>0.8</v>
@@ -4732,13 +4736,13 @@
     </row>
     <row r="17" ht="138.0" customHeight="1">
       <c r="A17" s="17" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
       <c r="L17" s="23"/>
       <c r="M17" s="23"/>
@@ -4765,7 +4769,7 @@
     </row>
     <row r="22">
       <c r="A22" s="34" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B22" s="34" t="s">
         <v>131</v>
@@ -5950,7 +5954,7 @@
         <v>146</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -6086,7 +6090,7 @@
         <v>120.0</v>
       </c>
       <c r="D7" s="11">
-        <f>AVERAGE(B7:C7)</f>
+        <f t="shared" ref="D7:D12" si="3">AVERAGE(B7:C7)</f>
         <v>99</v>
       </c>
       <c r="E7" s="10">
@@ -6110,13 +6114,16 @@
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
+      <c r="D8" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="E8" s="10">
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
       <c r="F8" s="10">
-        <f t="shared" ref="F8:F12" si="3">ROUND(F7*1.1,0)</f>
+        <f t="shared" ref="F8:F12" si="4">ROUND(F7*1.1,0)</f>
         <v>150</v>
       </c>
       <c r="G8" s="10">
@@ -6133,13 +6140,16 @@
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+      <c r="D9" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="E9" s="10">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
       <c r="F9" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>165</v>
       </c>
       <c r="G9" s="10">
@@ -6156,13 +6166,16 @@
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="D10" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="E10" s="10">
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
       <c r="F10" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>182</v>
       </c>
       <c r="G10" s="10">
@@ -6179,13 +6192,16 @@
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
+      <c r="D11" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="E11" s="10">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="F11" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>200</v>
       </c>
       <c r="G11" s="10">
@@ -6200,15 +6216,22 @@
       <c r="A12" s="10">
         <v>5.0</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
+      <c r="B12" s="10">
+        <v>100.0</v>
+      </c>
+      <c r="C12" s="10">
+        <v>211.0</v>
+      </c>
+      <c r="D12" s="11">
+        <f t="shared" si="3"/>
+        <v>155.5</v>
+      </c>
       <c r="E12" s="10">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
       <c r="F12" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>220</v>
       </c>
       <c r="G12" s="10">
@@ -6242,7 +6265,7 @@
         <v>95</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16">
@@ -6296,7 +6319,7 @@
         <v>102</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -6406,15 +6429,15 @@
       </c>
       <c r="E6" s="10">
         <f t="shared" ref="E6:E12" si="2">ROUND(F6*H6,0)</f>
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="F6" s="10">
         <f>ROUND(F7 * 0.9,0)</f>
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="G6" s="10">
         <f t="shared" ref="G6:G12" si="3">AVERAGE(E6:F6)</f>
-        <v>142.5</v>
+        <v>132</v>
       </c>
       <c r="H6" s="10">
         <v>0.65</v>
@@ -6436,14 +6459,14 @@
       </c>
       <c r="E7" s="10">
         <f t="shared" si="2"/>
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="F7" s="10">
-        <v>192.0</v>
+        <v>178.0</v>
       </c>
       <c r="G7" s="10">
         <f t="shared" si="3"/>
-        <v>158.5</v>
+        <v>147</v>
       </c>
       <c r="H7" s="10">
         <v>0.65</v>
@@ -6465,15 +6488,15 @@
       </c>
       <c r="E8" s="10">
         <f t="shared" si="2"/>
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="F8" s="10">
         <f t="shared" ref="F8:F12" si="4">ROUND(F7*1.1,0)</f>
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="G8" s="10">
         <f t="shared" si="3"/>
-        <v>174</v>
+        <v>161.5</v>
       </c>
       <c r="H8" s="10">
         <v>0.65</v>
@@ -6495,15 +6518,15 @@
       </c>
       <c r="E9" s="10">
         <f t="shared" si="2"/>
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="F9" s="10">
         <f t="shared" si="4"/>
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="G9" s="10">
         <f t="shared" si="3"/>
-        <v>191.5</v>
+        <v>178</v>
       </c>
       <c r="H9" s="10">
         <v>0.65</v>
@@ -6525,15 +6548,15 @@
       </c>
       <c r="E10" s="10">
         <f t="shared" si="2"/>
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="F10" s="10">
         <f t="shared" si="4"/>
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="G10" s="10">
         <f t="shared" si="3"/>
-        <v>210.5</v>
+        <v>196.5</v>
       </c>
       <c r="H10" s="10">
         <v>0.65</v>
@@ -6555,15 +6578,15 @@
       </c>
       <c r="E11" s="10">
         <f t="shared" si="2"/>
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="F11" s="10">
         <f t="shared" si="4"/>
-        <v>281</v>
+        <v>262</v>
       </c>
       <c r="G11" s="10">
         <f t="shared" si="3"/>
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="H11" s="10">
         <v>0.65</v>
@@ -6585,15 +6608,15 @@
       </c>
       <c r="E12" s="10">
         <f t="shared" si="2"/>
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="F12" s="10">
         <f t="shared" si="4"/>
-        <v>309</v>
+        <v>288</v>
       </c>
       <c r="G12" s="10">
         <f t="shared" si="3"/>
-        <v>255</v>
+        <v>237.5</v>
       </c>
       <c r="H12" s="10">
         <v>0.65</v>
@@ -6622,7 +6645,7 @@
         <v>95</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" ht="135.75" customHeight="1">
@@ -6667,13 +6690,13 @@
     </row>
     <row r="22">
       <c r="A22" s="34" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B22" s="34" t="s">
         <v>101</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>153</v>
@@ -7002,7 +7025,7 @@
         <v>95</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" ht="150.75" customHeight="1">
@@ -7985,7 +8008,7 @@
         <v>73</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -8040,7 +8063,7 @@
     </row>
     <row r="22">
       <c r="A22" s="34" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B22" s="34" t="s">
         <v>15</v>
@@ -8418,7 +8441,7 @@
         <v>145</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C22" s="34" t="s">
         <v>35</v>
@@ -8791,7 +8814,7 @@
     </row>
     <row r="22">
       <c r="A22" s="34" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B22" s="34" t="s">
         <v>102</v>
@@ -9184,7 +9207,7 @@
         <v>7</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>32</v>
@@ -9554,7 +9577,7 @@
         <v>101</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C22" s="23" t="s">
         <v>131</v>
@@ -9694,15 +9717,15 @@
       </c>
       <c r="E6" s="52">
         <f t="shared" ref="E6:E12" si="2">ROUND(F6*H6,0)</f>
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F6" s="52">
         <f>ROUND(F7 * 0.9,0)</f>
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="G6" s="52">
         <f t="shared" ref="G6:G12" si="3">AVERAGE(E6:F6)</f>
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="H6" s="51">
         <v>0.65</v>
@@ -9724,14 +9747,14 @@
       </c>
       <c r="E7" s="52">
         <f t="shared" si="2"/>
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F7" s="51">
-        <v>128.0</v>
+        <v>133.0</v>
       </c>
       <c r="G7" s="52">
         <f t="shared" si="3"/>
-        <v>105.5</v>
+        <v>109.5</v>
       </c>
       <c r="H7" s="51">
         <v>0.65</v>
@@ -9753,15 +9776,15 @@
       </c>
       <c r="E8" s="52">
         <f t="shared" si="2"/>
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F8" s="52">
         <f t="shared" ref="F8:F12" si="4">ROUND(F7*1.1,0)</f>
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="G8" s="52">
         <f t="shared" si="3"/>
-        <v>116.5</v>
+        <v>120.5</v>
       </c>
       <c r="H8" s="51">
         <v>0.65</v>
@@ -9784,15 +9807,15 @@
       </c>
       <c r="E9" s="52">
         <f t="shared" si="2"/>
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="F9" s="52">
         <f t="shared" si="4"/>
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="G9" s="52">
         <f t="shared" si="3"/>
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="H9" s="51">
         <v>0.65</v>
@@ -9814,15 +9837,15 @@
       </c>
       <c r="E10" s="52">
         <f t="shared" si="2"/>
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="F10" s="52">
         <f t="shared" si="4"/>
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="G10" s="52">
         <f t="shared" si="3"/>
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="H10" s="51">
         <v>0.65</v>
@@ -9844,15 +9867,15 @@
       </c>
       <c r="E11" s="52">
         <f t="shared" si="2"/>
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="F11" s="52">
         <f t="shared" si="4"/>
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="G11" s="52">
         <f t="shared" si="3"/>
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="H11" s="51">
         <v>0.65</v>
@@ -9874,15 +9897,15 @@
       </c>
       <c r="E12" s="52">
         <f t="shared" si="2"/>
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="F12" s="52">
         <f t="shared" si="4"/>
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="G12" s="52">
         <f t="shared" si="3"/>
-        <v>171</v>
+        <v>177.5</v>
       </c>
       <c r="H12" s="51">
         <v>0.65</v>
@@ -9920,10 +9943,10 @@
         <v>84</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20">
@@ -10078,15 +10101,15 @@
       </c>
       <c r="E6" s="52">
         <f t="shared" ref="E6:E12" si="2">ROUND(F6*H6,0)</f>
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F6" s="52">
         <f>ROUND(F7 * 0.9,0)</f>
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="G6" s="52">
         <f t="shared" ref="G6:G12" si="3">AVERAGE(E6:F6)</f>
-        <v>67.5</v>
+        <v>72</v>
       </c>
       <c r="H6" s="51">
         <v>0.8</v>
@@ -10108,14 +10131,14 @@
       </c>
       <c r="E7" s="52">
         <f t="shared" si="2"/>
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="F7" s="51">
-        <v>83.0</v>
+        <v>89.0</v>
       </c>
       <c r="G7" s="52">
         <f t="shared" si="3"/>
-        <v>74.5</v>
+        <v>80</v>
       </c>
       <c r="H7" s="51">
         <v>0.8</v>
@@ -10137,15 +10160,15 @@
       </c>
       <c r="E8" s="52">
         <f t="shared" si="2"/>
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F8" s="52">
         <f t="shared" ref="F8:F12" si="4">ROUND(F7*1.1,0)</f>
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="G8" s="52">
         <f t="shared" si="3"/>
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="H8" s="51">
         <v>0.8</v>
@@ -10168,15 +10191,15 @@
       </c>
       <c r="E9" s="52">
         <f t="shared" si="2"/>
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F9" s="52">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="G9" s="52">
         <f t="shared" si="3"/>
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="H9" s="51">
         <v>0.8</v>
@@ -10198,15 +10221,15 @@
       </c>
       <c r="E10" s="52">
         <f t="shared" si="2"/>
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="F10" s="52">
         <f t="shared" si="4"/>
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="G10" s="52">
         <f t="shared" si="3"/>
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="H10" s="51">
         <v>0.8</v>
@@ -10228,15 +10251,15 @@
       </c>
       <c r="E11" s="52">
         <f t="shared" si="2"/>
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="F11" s="52">
         <f t="shared" si="4"/>
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="G11" s="52">
         <f t="shared" si="3"/>
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="H11" s="51">
         <v>0.8</v>
@@ -10258,15 +10281,15 @@
       </c>
       <c r="E12" s="52">
         <f t="shared" si="2"/>
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="F12" s="52">
         <f t="shared" si="4"/>
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="G12" s="52">
         <f t="shared" si="3"/>
-        <v>119.5</v>
+        <v>129.5</v>
       </c>
       <c r="H12" s="51">
         <v>0.8</v>
@@ -11061,7 +11084,7 @@
         <v>95</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" ht="109.5" customHeight="1">
@@ -13741,13 +13764,13 @@
         <v>105</v>
       </c>
       <c r="B22" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="27" t="s">
+      <c r="D22" s="14" t="s">
         <v>107</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>